<commit_message>
Update measurement scripts with live plotting. Correct gates.
</commit_message>
<xml_diff>
--- a/DCMapping.xlsx
+++ b/DCMapping.xlsx
@@ -234,7 +234,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="10"/>
@@ -259,10 +259,6 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="7" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="11" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="3" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="9" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="11" applyFill="1"/>
   </cellXfs>
@@ -564,11 +560,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K115"/>
+  <dimension ref="A1:K113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L67" sqref="L67"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A80" sqref="A79:K80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1827,7 +1823,7 @@
       </c>
       <c r="I57" s="11"/>
       <c r="J57" s="11"/>
-      <c r="K57" s="28">
+      <c r="K57" s="24">
         <v>1</v>
       </c>
     </row>
@@ -1848,7 +1844,7 @@
       </c>
       <c r="I58" s="11"/>
       <c r="J58" s="11"/>
-      <c r="K58" s="28">
+      <c r="K58" s="24">
         <v>14</v>
       </c>
     </row>
@@ -1870,7 +1866,7 @@
       </c>
       <c r="I59" s="11"/>
       <c r="J59" s="11"/>
-      <c r="K59" s="28">
+      <c r="K59" s="24">
         <f>K57+1</f>
         <v>2</v>
       </c>
@@ -1893,7 +1889,7 @@
       </c>
       <c r="I60" s="11"/>
       <c r="J60" s="11"/>
-      <c r="K60" s="28">
+      <c r="K60" s="24">
         <f>K58+1</f>
         <v>15</v>
       </c>
@@ -1916,7 +1912,7 @@
       </c>
       <c r="I61" s="11"/>
       <c r="J61" s="11"/>
-      <c r="K61" s="28">
+      <c r="K61" s="24">
         <f t="shared" ref="K61:K73" si="6">K59+1</f>
         <v>3</v>
       </c>
@@ -1939,7 +1935,7 @@
       </c>
       <c r="I62" s="11"/>
       <c r="J62" s="11"/>
-      <c r="K62" s="28">
+      <c r="K62" s="24">
         <f t="shared" si="6"/>
         <v>16</v>
       </c>
@@ -1962,7 +1958,7 @@
       </c>
       <c r="I63" s="11"/>
       <c r="J63" s="11"/>
-      <c r="K63" s="28">
+      <c r="K63" s="24">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
@@ -1985,7 +1981,7 @@
       </c>
       <c r="I64" s="11"/>
       <c r="J64" s="11"/>
-      <c r="K64" s="28">
+      <c r="K64" s="24">
         <f t="shared" si="6"/>
         <v>17</v>
       </c>
@@ -2008,7 +2004,7 @@
       </c>
       <c r="I65" s="11"/>
       <c r="J65" s="11"/>
-      <c r="K65" s="28">
+      <c r="K65" s="24">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
@@ -2031,7 +2027,7 @@
       </c>
       <c r="I66" s="11"/>
       <c r="J66" s="11"/>
-      <c r="K66" s="28">
+      <c r="K66" s="24">
         <f t="shared" si="6"/>
         <v>18</v>
       </c>
@@ -2054,7 +2050,7 @@
       </c>
       <c r="I67" s="11"/>
       <c r="J67" s="11"/>
-      <c r="K67" s="28">
+      <c r="K67" s="24">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
@@ -2077,7 +2073,7 @@
       </c>
       <c r="I68" s="11"/>
       <c r="J68" s="11"/>
-      <c r="K68" s="28">
+      <c r="K68" s="24">
         <f t="shared" si="6"/>
         <v>19</v>
       </c>
@@ -2100,7 +2096,7 @@
       </c>
       <c r="I69" s="11"/>
       <c r="J69" s="11"/>
-      <c r="K69" s="28">
+      <c r="K69" s="24">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
@@ -2123,7 +2119,7 @@
       </c>
       <c r="I70" s="11"/>
       <c r="J70" s="11"/>
-      <c r="K70" s="28">
+      <c r="K70" s="24">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
@@ -2146,7 +2142,7 @@
       </c>
       <c r="I71" s="11"/>
       <c r="J71" s="11"/>
-      <c r="K71" s="28">
+      <c r="K71" s="24">
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
@@ -2169,7 +2165,7 @@
       </c>
       <c r="I72" s="11"/>
       <c r="J72" s="11"/>
-      <c r="K72" s="28">
+      <c r="K72" s="24">
         <f t="shared" si="6"/>
         <v>21</v>
       </c>
@@ -2183,7 +2179,7 @@
       </c>
       <c r="C73" s="11"/>
       <c r="D73" s="7">
-        <f t="shared" ref="D73:D105" si="7">D72+1</f>
+        <f t="shared" ref="D73:D104" si="7">D72+1</f>
         <v>68</v>
       </c>
       <c r="G73" s="8">
@@ -2192,7 +2188,7 @@
       </c>
       <c r="I73" s="11"/>
       <c r="J73" s="11"/>
-      <c r="K73" s="28">
+      <c r="K73" s="24">
         <f t="shared" si="6"/>
         <v>9</v>
       </c>
@@ -2215,7 +2211,7 @@
       </c>
       <c r="I74" s="11"/>
       <c r="J74" s="11"/>
-      <c r="K74" s="28">
+      <c r="K74" s="24">
         <f>K72+1</f>
         <v>22</v>
       </c>
@@ -2238,7 +2234,7 @@
       </c>
       <c r="I75" s="11"/>
       <c r="J75" s="11"/>
-      <c r="K75" s="28">
+      <c r="K75" s="24">
         <f>K73+1</f>
         <v>10</v>
       </c>
@@ -2261,7 +2257,7 @@
       </c>
       <c r="I76" s="11"/>
       <c r="J76" s="11"/>
-      <c r="K76" s="28">
+      <c r="K76" s="24">
         <f t="shared" ref="K76:K79" si="9">K74+1</f>
         <v>23</v>
       </c>
@@ -2284,7 +2280,7 @@
       </c>
       <c r="I77" s="11"/>
       <c r="J77" s="11"/>
-      <c r="K77" s="28">
+      <c r="K77" s="24">
         <f t="shared" si="9"/>
         <v>11</v>
       </c>
@@ -2307,7 +2303,7 @@
       </c>
       <c r="I78" s="11"/>
       <c r="J78" s="11"/>
-      <c r="K78" s="28">
+      <c r="K78" s="24">
         <f t="shared" si="9"/>
         <v>24</v>
       </c>
@@ -2330,7 +2326,7 @@
       </c>
       <c r="I79" s="11"/>
       <c r="J79" s="11"/>
-      <c r="K79" s="28">
+      <c r="K79" s="24">
         <f t="shared" si="9"/>
         <v>12</v>
       </c>
@@ -2353,623 +2349,629 @@
       </c>
       <c r="I80" s="11"/>
       <c r="J80" s="11"/>
-      <c r="K80" s="19"/>
+      <c r="K80" s="24">
+        <v>13</v>
+      </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="24"/>
-      <c r="B81" s="25"/>
-      <c r="C81" s="25"/>
-      <c r="D81" s="26"/>
-      <c r="E81" s="25"/>
-      <c r="F81" s="25"/>
-      <c r="G81" s="27"/>
-      <c r="H81" s="25"/>
-      <c r="I81" s="25"/>
-      <c r="J81" s="25"/>
-      <c r="K81" s="28">
+      <c r="A81" s="17"/>
+      <c r="B81" s="16"/>
+      <c r="C81" s="16"/>
+      <c r="D81" s="20"/>
+      <c r="E81" s="16"/>
+      <c r="F81" s="16"/>
+      <c r="G81" s="8">
         <v>13</v>
       </c>
+      <c r="H81" s="16"/>
+      <c r="I81" s="16"/>
+      <c r="J81" s="16"/>
+      <c r="K81" s="16"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" s="17"/>
-      <c r="B82" s="16"/>
-      <c r="C82" s="16"/>
-      <c r="D82" s="20"/>
-      <c r="E82" s="16"/>
-      <c r="F82" s="16"/>
-      <c r="G82" s="8">
-        <v>13</v>
-      </c>
-      <c r="H82" s="16"/>
-      <c r="I82" s="16"/>
-      <c r="J82" s="16"/>
-      <c r="K82" s="16"/>
+      <c r="A82" s="6">
+        <v>24</v>
+      </c>
+      <c r="B82" s="11">
+        <v>24</v>
+      </c>
+      <c r="C82" s="10"/>
+      <c r="D82" s="7">
+        <f>D80+1</f>
+        <v>76</v>
+      </c>
+      <c r="H82" s="8">
+        <v>1</v>
+      </c>
+      <c r="I82" s="11"/>
+      <c r="J82" s="14"/>
+      <c r="K82" s="25">
+        <f>H82+24</f>
+        <v>25</v>
+      </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="6">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B83" s="11">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C83" s="10"/>
       <c r="D83" s="7">
-        <f>D80+1</f>
-        <v>76</v>
+        <f t="shared" si="7"/>
+        <v>77</v>
       </c>
       <c r="H83" s="8">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="I83" s="11"/>
       <c r="J83" s="14"/>
-      <c r="K83" s="15">
-        <f>H83+24</f>
-        <v>25</v>
+      <c r="K83" s="25">
+        <f t="shared" ref="K83:K104" si="10">H83+24</f>
+        <v>38</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="6">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B84" s="11">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C84" s="10"/>
       <c r="D84" s="7">
         <f t="shared" si="7"/>
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H84" s="8">
-        <v>14</v>
+        <f>H82+1</f>
+        <v>2</v>
       </c>
       <c r="I84" s="11"/>
       <c r="J84" s="14"/>
-      <c r="K84" s="29">
-        <f t="shared" ref="K84:K105" si="10">H84+24</f>
-        <v>38</v>
+      <c r="K84" s="25">
+        <f t="shared" si="10"/>
+        <v>26</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="6">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B85" s="11">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C85" s="10"/>
       <c r="D85" s="7">
         <f t="shared" si="7"/>
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H85" s="8">
         <f>H83+1</f>
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I85" s="11"/>
       <c r="J85" s="14"/>
-      <c r="K85" s="29">
+      <c r="K85" s="25">
         <f t="shared" si="10"/>
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="6">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B86" s="11">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C86" s="10"/>
       <c r="D86" s="7">
         <f t="shared" si="7"/>
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H86" s="8">
-        <f>H84+1</f>
-        <v>15</v>
+        <f t="shared" ref="H86:H105" si="11">H84+1</f>
+        <v>3</v>
       </c>
       <c r="I86" s="11"/>
       <c r="J86" s="14"/>
-      <c r="K86" s="29">
+      <c r="K86" s="25">
         <f t="shared" si="10"/>
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="6">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B87" s="11">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C87" s="10"/>
       <c r="D87" s="7">
         <f t="shared" si="7"/>
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H87" s="8">
-        <f t="shared" ref="H87:H106" si="11">H85+1</f>
-        <v>3</v>
+        <f t="shared" si="11"/>
+        <v>16</v>
       </c>
       <c r="I87" s="11"/>
       <c r="J87" s="14"/>
-      <c r="K87" s="29">
+      <c r="K87" s="25">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="6">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B88" s="11">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C88" s="10"/>
       <c r="D88" s="7">
         <f t="shared" si="7"/>
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H88" s="8">
         <f t="shared" si="11"/>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I88" s="11"/>
       <c r="J88" s="14"/>
-      <c r="K88" s="29">
+      <c r="K88" s="25">
         <f t="shared" si="10"/>
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="6">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B89" s="11">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C89" s="10"/>
       <c r="D89" s="7">
         <f t="shared" si="7"/>
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H89" s="8">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="I89" s="11"/>
       <c r="J89" s="14"/>
-      <c r="K89" s="29">
+      <c r="K89" s="25">
         <f t="shared" si="10"/>
-        <v>28</v>
+        <v>41</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="6">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B90" s="11">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C90" s="10"/>
       <c r="D90" s="7">
         <f t="shared" si="7"/>
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H90" s="8">
         <f t="shared" si="11"/>
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="I90" s="11"/>
       <c r="J90" s="14"/>
-      <c r="K90" s="29">
+      <c r="K90" s="25">
         <f t="shared" si="10"/>
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="6">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B91" s="11">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C91" s="10"/>
       <c r="D91" s="7">
         <f t="shared" si="7"/>
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H91" s="8">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="I91" s="11"/>
       <c r="J91" s="14"/>
-      <c r="K91" s="29">
+      <c r="K91" s="25">
         <f t="shared" si="10"/>
-        <v>29</v>
+        <v>42</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="6">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B92" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C92" s="10"/>
       <c r="D92" s="7">
         <f t="shared" si="7"/>
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H92" s="8">
         <f t="shared" si="11"/>
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="I92" s="11"/>
       <c r="J92" s="14"/>
-      <c r="K92" s="29">
+      <c r="K92" s="25">
         <f t="shared" si="10"/>
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="6">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B93" s="11">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C93" s="10"/>
       <c r="D93" s="7">
         <f t="shared" si="7"/>
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H93" s="8">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="I93" s="11"/>
       <c r="J93" s="14"/>
-      <c r="K93" s="29">
+      <c r="K93" s="25">
         <f t="shared" si="10"/>
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B94" s="11">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="7">
         <f t="shared" si="7"/>
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H94" s="8">
         <f t="shared" si="11"/>
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="I94" s="11"/>
       <c r="J94" s="14"/>
-      <c r="K94" s="29">
+      <c r="K94" s="25">
         <f t="shared" si="10"/>
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="6">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B95" s="11">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C95" s="10"/>
       <c r="D95" s="7">
         <f t="shared" si="7"/>
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H95" s="8">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I95" s="11"/>
       <c r="J95" s="14"/>
-      <c r="K95" s="29">
+      <c r="K95" s="25">
         <f t="shared" si="10"/>
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="6">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B96" s="11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C96" s="10"/>
       <c r="D96" s="7">
         <f t="shared" si="7"/>
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H96" s="8">
         <f t="shared" si="11"/>
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="I96" s="11"/>
       <c r="J96" s="14"/>
-      <c r="K96" s="29">
+      <c r="K96" s="25">
         <f t="shared" si="10"/>
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="6">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B97" s="11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C97" s="10"/>
       <c r="D97" s="7">
         <f t="shared" si="7"/>
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H97" s="8">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="I97" s="11"/>
       <c r="J97" s="14"/>
-      <c r="K97" s="29">
+      <c r="K97" s="25">
         <f t="shared" si="10"/>
-        <v>32</v>
+        <v>45</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B98" s="11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C98" s="10"/>
       <c r="D98" s="7">
         <f t="shared" si="7"/>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H98" s="8">
         <f t="shared" si="11"/>
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="I98" s="11"/>
       <c r="J98" s="14"/>
-      <c r="K98" s="29">
+      <c r="K98" s="25">
         <f t="shared" si="10"/>
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B99" s="11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C99" s="10"/>
       <c r="D99" s="7">
         <f t="shared" si="7"/>
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H99" s="8">
         <f t="shared" si="11"/>
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I99" s="11"/>
       <c r="J99" s="14"/>
-      <c r="K99" s="29">
+      <c r="K99" s="25">
         <f t="shared" si="10"/>
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B100" s="11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C100" s="10"/>
       <c r="D100" s="7">
         <f t="shared" si="7"/>
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H100" s="8">
         <f t="shared" si="11"/>
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I100" s="11"/>
       <c r="J100" s="14"/>
-      <c r="K100" s="29">
+      <c r="K100" s="25">
         <f t="shared" si="10"/>
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B101" s="11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C101" s="10"/>
       <c r="D101" s="7">
         <f t="shared" si="7"/>
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H101" s="8">
         <f t="shared" si="11"/>
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="I101" s="11"/>
       <c r="J101" s="14"/>
-      <c r="K101" s="29">
+      <c r="K101" s="25">
         <f t="shared" si="10"/>
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B102" s="11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C102" s="10"/>
       <c r="D102" s="7">
         <f t="shared" si="7"/>
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H102" s="8">
         <f t="shared" si="11"/>
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="I102" s="11"/>
       <c r="J102" s="14"/>
-      <c r="K102" s="29">
+      <c r="K102" s="25">
         <f t="shared" si="10"/>
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B103" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C103" s="10"/>
       <c r="D103" s="7">
         <f t="shared" si="7"/>
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H103" s="8">
         <f t="shared" si="11"/>
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="I103" s="11"/>
       <c r="J103" s="14"/>
-      <c r="K103" s="29">
+      <c r="K103" s="25">
         <f t="shared" si="10"/>
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B104" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C104" s="10"/>
       <c r="D104" s="7">
         <f t="shared" si="7"/>
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H104" s="8">
         <f t="shared" si="11"/>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="I104" s="11"/>
       <c r="J104" s="14"/>
-      <c r="K104" s="29">
+      <c r="K104" s="25">
         <f t="shared" si="10"/>
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B105" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C105" s="10"/>
       <c r="D105" s="7">
-        <f t="shared" si="7"/>
-        <v>98</v>
+        <f>D104+1</f>
+        <v>99</v>
       </c>
       <c r="H105" s="8">
         <f t="shared" si="11"/>
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="I105" s="11"/>
       <c r="J105" s="14"/>
-      <c r="K105" s="29">
-        <f t="shared" si="10"/>
-        <v>36</v>
+      <c r="K105" s="25">
+        <v>37</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A106" s="6">
-        <v>1</v>
-      </c>
-      <c r="B106" s="11">
-        <v>1</v>
-      </c>
-      <c r="C106" s="10"/>
-      <c r="D106" s="7">
-        <f>D105+1</f>
-        <v>99</v>
-      </c>
+      <c r="A106" s="17"/>
+      <c r="B106" s="16"/>
+      <c r="C106" s="18"/>
+      <c r="D106" s="20"/>
+      <c r="E106" s="16"/>
+      <c r="F106" s="16"/>
+      <c r="G106" s="16"/>
       <c r="H106" s="8">
-        <f t="shared" si="11"/>
-        <v>25</v>
-      </c>
-      <c r="I106" s="11"/>
-      <c r="J106" s="14"/>
+        <v>13</v>
+      </c>
+      <c r="I106" s="16"/>
+      <c r="J106" s="21"/>
       <c r="K106" s="22"/>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="17"/>
       <c r="B107" s="16"/>
       <c r="C107" s="18"/>
-      <c r="D107" s="20"/>
+      <c r="D107" s="7">
+        <f>D105+1</f>
+        <v>100</v>
+      </c>
       <c r="E107" s="16"/>
       <c r="F107" s="16"/>
       <c r="G107" s="16"/>
-      <c r="H107" s="19"/>
+      <c r="H107" s="16"/>
       <c r="I107" s="16"/>
-      <c r="J107" s="21"/>
-      <c r="K107" s="29">
-        <v>37</v>
-      </c>
+      <c r="J107" s="16"/>
+      <c r="K107" s="16"/>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A108" s="17"/>
-      <c r="B108" s="16"/>
-      <c r="C108" s="18"/>
-      <c r="D108" s="20"/>
+      <c r="A108" s="12">
+        <v>49</v>
+      </c>
+      <c r="B108" s="11">
+        <v>49</v>
+      </c>
+      <c r="D108" s="16"/>
       <c r="E108" s="16"/>
       <c r="F108" s="16"/>
       <c r="G108" s="16"/>
-      <c r="H108" s="8">
-        <v>13</v>
-      </c>
+      <c r="H108" s="16"/>
       <c r="I108" s="16"/>
-      <c r="J108" s="21"/>
-      <c r="K108" s="22"/>
+      <c r="J108" s="16"/>
+      <c r="K108" s="16"/>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A109" s="17"/>
-      <c r="B109" s="16"/>
-      <c r="C109" s="18"/>
-      <c r="D109" s="7">
-        <f>D106+1</f>
-        <v>100</v>
-      </c>
+      <c r="A109" s="12">
+        <v>50</v>
+      </c>
+      <c r="B109">
+        <v>50</v>
+      </c>
+      <c r="D109" s="16"/>
       <c r="E109" s="16"/>
       <c r="F109" s="16"/>
       <c r="G109" s="16"/>
@@ -2980,10 +2982,10 @@
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="12">
-        <v>49</v>
-      </c>
-      <c r="B110" s="11">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="B110">
+        <v>51</v>
       </c>
       <c r="D110" s="16"/>
       <c r="E110" s="16"/>
@@ -2996,10 +2998,10 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="12">
-        <v>50</v>
-      </c>
-      <c r="B111">
-        <v>50</v>
+        <v>100</v>
+      </c>
+      <c r="C111">
+        <v>49</v>
       </c>
       <c r="D111" s="16"/>
       <c r="E111" s="16"/>
@@ -3012,10 +3014,10 @@
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="12">
-        <v>51</v>
-      </c>
-      <c r="B112">
-        <v>51</v>
+        <v>101</v>
+      </c>
+      <c r="C112">
+        <v>50</v>
       </c>
       <c r="D112" s="16"/>
       <c r="E112" s="16"/>
@@ -3027,11 +3029,11 @@
       <c r="K112" s="16"/>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A113" s="12">
-        <v>100</v>
+      <c r="A113" s="13">
+        <v>102</v>
       </c>
       <c r="C113">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D113" s="16"/>
       <c r="E113" s="16"/>
@@ -3042,44 +3044,12 @@
       <c r="J113" s="16"/>
       <c r="K113" s="16"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A114" s="12">
-        <v>101</v>
-      </c>
-      <c r="C114">
-        <v>50</v>
-      </c>
-      <c r="D114" s="16"/>
-      <c r="E114" s="16"/>
-      <c r="F114" s="16"/>
-      <c r="G114" s="16"/>
-      <c r="H114" s="16"/>
-      <c r="I114" s="16"/>
-      <c r="J114" s="16"/>
-      <c r="K114" s="16"/>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A115" s="13">
-        <v>102</v>
-      </c>
-      <c r="C115">
-        <v>51</v>
-      </c>
-      <c r="D115" s="16"/>
-      <c r="E115" s="16"/>
-      <c r="F115" s="16"/>
-      <c r="G115" s="16"/>
-      <c r="H115" s="16"/>
-      <c r="I115" s="16"/>
-      <c r="J115" s="16"/>
-      <c r="K115" s="16"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="45" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="109" max="16383" man="1"/>
+    <brk id="107" max="16383" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="11" max="1048575" man="1"/>

</xml_diff>

<commit_message>
Mapping from bottom of fridge added
</commit_message>
<xml_diff>
--- a/DCMapping.xlsx
+++ b/DCMapping.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TOP" sheetId="1" r:id="rId1"/>
+    <sheet name="BOT" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>DBA pads</t>
   </si>
@@ -61,12 +62,33 @@
   <si>
     <t>NanoD 51 2</t>
   </si>
+  <si>
+    <t>Micro-d 25 1 Bot</t>
+  </si>
+  <si>
+    <t>Micro-d 25 2 Bot</t>
+  </si>
+  <si>
+    <t>MicroD 51 Bot 1</t>
+  </si>
+  <si>
+    <t>MicroD 51 Bot 3</t>
+  </si>
+  <si>
+    <t>Micro-d 25 5 Bot</t>
+  </si>
+  <si>
+    <t>Micro-d 25 6 Bot</t>
+  </si>
+  <si>
+    <t>MDAC SMC Bot</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -103,8 +125,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,6 +235,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8181"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -234,7 +286,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="10"/>
@@ -261,6 +313,23 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="11" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="8" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="12" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="9" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="9" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -283,6 +352,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF8181"/>
       <color rgb="FFFFB9B9"/>
     </mruColors>
   </colors>
@@ -563,8 +633,8 @@
   <dimension ref="A1:K113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A80" sqref="A79:K80"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -583,10 +653,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="42" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -619,7 +689,7 @@
         <v>52</v>
       </c>
       <c r="B2" s="10"/>
-      <c r="C2" s="11">
+      <c r="C2" s="41">
         <v>1</v>
       </c>
       <c r="D2" s="7">
@@ -639,7 +709,7 @@
         <v>53</v>
       </c>
       <c r="B3" s="10"/>
-      <c r="C3" s="11">
+      <c r="C3" s="41">
         <v>2</v>
       </c>
       <c r="D3" s="7">
@@ -659,7 +729,7 @@
         <v>54</v>
       </c>
       <c r="B4" s="10"/>
-      <c r="C4" s="11">
+      <c r="C4" s="41">
         <v>3</v>
       </c>
       <c r="D4" s="7">
@@ -680,7 +750,7 @@
         <v>55</v>
       </c>
       <c r="B5" s="10"/>
-      <c r="C5" s="11">
+      <c r="C5" s="41">
         <v>4</v>
       </c>
       <c r="D5" s="7">
@@ -701,7 +771,7 @@
         <v>56</v>
       </c>
       <c r="B6" s="10"/>
-      <c r="C6" s="11">
+      <c r="C6" s="41">
         <v>5</v>
       </c>
       <c r="D6" s="7">
@@ -722,7 +792,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="41">
         <v>6</v>
       </c>
       <c r="D7" s="7">
@@ -743,7 +813,7 @@
         <v>58</v>
       </c>
       <c r="B8" s="10"/>
-      <c r="C8" s="11">
+      <c r="C8" s="41">
         <v>7</v>
       </c>
       <c r="D8" s="7">
@@ -766,7 +836,7 @@
         <v>59</v>
       </c>
       <c r="B9" s="10"/>
-      <c r="C9" s="11">
+      <c r="C9" s="41">
         <v>8</v>
       </c>
       <c r="D9" s="7">
@@ -789,7 +859,7 @@
         <v>60</v>
       </c>
       <c r="B10" s="10"/>
-      <c r="C10" s="11">
+      <c r="C10" s="41">
         <v>9</v>
       </c>
       <c r="D10" s="7">
@@ -812,7 +882,7 @@
         <v>61</v>
       </c>
       <c r="B11" s="10"/>
-      <c r="C11" s="11">
+      <c r="C11" s="41">
         <v>10</v>
       </c>
       <c r="D11" s="7">
@@ -835,7 +905,7 @@
         <v>62</v>
       </c>
       <c r="B12" s="10"/>
-      <c r="C12" s="11">
+      <c r="C12" s="41">
         <v>11</v>
       </c>
       <c r="D12" s="7">
@@ -858,7 +928,7 @@
         <v>63</v>
       </c>
       <c r="B13" s="10"/>
-      <c r="C13" s="11">
+      <c r="C13" s="41">
         <v>12</v>
       </c>
       <c r="D13" s="7">
@@ -881,7 +951,7 @@
         <v>64</v>
       </c>
       <c r="B14" s="10"/>
-      <c r="C14" s="11">
+      <c r="C14" s="41">
         <v>13</v>
       </c>
       <c r="D14" s="7">
@@ -904,7 +974,7 @@
         <v>65</v>
       </c>
       <c r="B15" s="10"/>
-      <c r="C15" s="11">
+      <c r="C15" s="41">
         <v>14</v>
       </c>
       <c r="D15" s="7">
@@ -927,7 +997,7 @@
         <v>66</v>
       </c>
       <c r="B16" s="10"/>
-      <c r="C16" s="11">
+      <c r="C16" s="41">
         <v>15</v>
       </c>
       <c r="D16" s="7">
@@ -950,7 +1020,7 @@
         <v>67</v>
       </c>
       <c r="B17" s="10"/>
-      <c r="C17" s="11">
+      <c r="C17" s="41">
         <v>16</v>
       </c>
       <c r="D17" s="7">
@@ -973,7 +1043,7 @@
         <v>68</v>
       </c>
       <c r="B18" s="10"/>
-      <c r="C18" s="11">
+      <c r="C18" s="41">
         <v>17</v>
       </c>
       <c r="D18" s="7">
@@ -996,7 +1066,7 @@
         <v>69</v>
       </c>
       <c r="B19" s="10"/>
-      <c r="C19" s="11">
+      <c r="C19" s="41">
         <v>18</v>
       </c>
       <c r="D19" s="7">
@@ -1019,7 +1089,7 @@
         <v>70</v>
       </c>
       <c r="B20" s="10"/>
-      <c r="C20" s="11">
+      <c r="C20" s="41">
         <v>19</v>
       </c>
       <c r="D20" s="7">
@@ -1042,7 +1112,7 @@
         <v>71</v>
       </c>
       <c r="B21" s="10"/>
-      <c r="C21" s="11">
+      <c r="C21" s="41">
         <v>20</v>
       </c>
       <c r="D21" s="7">
@@ -1065,7 +1135,7 @@
         <v>72</v>
       </c>
       <c r="B22" s="10"/>
-      <c r="C22" s="11">
+      <c r="C22" s="41">
         <v>21</v>
       </c>
       <c r="D22" s="7">
@@ -1088,7 +1158,7 @@
         <v>73</v>
       </c>
       <c r="B23" s="10"/>
-      <c r="C23" s="11">
+      <c r="C23" s="41">
         <v>22</v>
       </c>
       <c r="D23" s="7">
@@ -1111,7 +1181,7 @@
         <v>74</v>
       </c>
       <c r="B24" s="10"/>
-      <c r="C24" s="11">
+      <c r="C24" s="41">
         <v>23</v>
       </c>
       <c r="D24" s="7">
@@ -1134,7 +1204,7 @@
         <v>75</v>
       </c>
       <c r="B25" s="10"/>
-      <c r="C25" s="11">
+      <c r="C25" s="41">
         <v>24</v>
       </c>
       <c r="D25" s="7">
@@ -1219,7 +1289,7 @@
         <v>76</v>
       </c>
       <c r="B30" s="11"/>
-      <c r="C30" s="11">
+      <c r="C30" s="38">
         <v>25</v>
       </c>
       <c r="D30" s="7">
@@ -1240,7 +1310,7 @@
         <v>77</v>
       </c>
       <c r="B31" s="11"/>
-      <c r="C31" s="11">
+      <c r="C31" s="38">
         <v>26</v>
       </c>
       <c r="D31" s="7">
@@ -1261,7 +1331,7 @@
         <v>78</v>
       </c>
       <c r="B32" s="11"/>
-      <c r="C32" s="11">
+      <c r="C32" s="38">
         <v>27</v>
       </c>
       <c r="D32" s="7">
@@ -1284,7 +1354,7 @@
         <v>79</v>
       </c>
       <c r="B33" s="11"/>
-      <c r="C33" s="11">
+      <c r="C33" s="38">
         <v>28</v>
       </c>
       <c r="D33" s="7">
@@ -1307,7 +1377,7 @@
         <v>80</v>
       </c>
       <c r="B34" s="11"/>
-      <c r="C34" s="11">
+      <c r="C34" s="38">
         <v>29</v>
       </c>
       <c r="D34" s="7">
@@ -1330,7 +1400,7 @@
         <v>81</v>
       </c>
       <c r="B35" s="11"/>
-      <c r="C35" s="11">
+      <c r="C35" s="38">
         <v>30</v>
       </c>
       <c r="D35" s="7">
@@ -1353,7 +1423,7 @@
         <v>82</v>
       </c>
       <c r="B36" s="11"/>
-      <c r="C36" s="11">
+      <c r="C36" s="38">
         <v>31</v>
       </c>
       <c r="D36" s="7">
@@ -1376,7 +1446,7 @@
         <v>83</v>
       </c>
       <c r="B37" s="11"/>
-      <c r="C37" s="11">
+      <c r="C37" s="38">
         <v>32</v>
       </c>
       <c r="D37" s="7">
@@ -1399,7 +1469,7 @@
         <v>84</v>
       </c>
       <c r="B38" s="11"/>
-      <c r="C38" s="11">
+      <c r="C38" s="38">
         <v>33</v>
       </c>
       <c r="D38" s="7">
@@ -1422,7 +1492,7 @@
         <v>85</v>
       </c>
       <c r="B39" s="11"/>
-      <c r="C39" s="11">
+      <c r="C39" s="38">
         <v>34</v>
       </c>
       <c r="D39" s="7">
@@ -1445,7 +1515,7 @@
         <v>86</v>
       </c>
       <c r="B40" s="11"/>
-      <c r="C40" s="11">
+      <c r="C40" s="38">
         <v>35</v>
       </c>
       <c r="D40" s="7">
@@ -1468,7 +1538,7 @@
         <v>87</v>
       </c>
       <c r="B41" s="11"/>
-      <c r="C41" s="11">
+      <c r="C41" s="38">
         <v>36</v>
       </c>
       <c r="D41" s="7">
@@ -1491,7 +1561,7 @@
         <v>88</v>
       </c>
       <c r="B42" s="11"/>
-      <c r="C42" s="11">
+      <c r="C42" s="38">
         <v>37</v>
       </c>
       <c r="D42" s="7">
@@ -1514,7 +1584,7 @@
         <v>89</v>
       </c>
       <c r="B43" s="11"/>
-      <c r="C43" s="11">
+      <c r="C43" s="38">
         <v>38</v>
       </c>
       <c r="D43" s="7">
@@ -1537,7 +1607,7 @@
         <v>90</v>
       </c>
       <c r="B44" s="11"/>
-      <c r="C44" s="11">
+      <c r="C44" s="38">
         <v>39</v>
       </c>
       <c r="D44" s="7">
@@ -1560,7 +1630,7 @@
         <v>91</v>
       </c>
       <c r="B45" s="11"/>
-      <c r="C45" s="11">
+      <c r="C45" s="38">
         <v>40</v>
       </c>
       <c r="D45" s="7">
@@ -1583,7 +1653,7 @@
         <v>92</v>
       </c>
       <c r="B46" s="11"/>
-      <c r="C46" s="11">
+      <c r="C46" s="38">
         <v>41</v>
       </c>
       <c r="D46" s="7">
@@ -1606,7 +1676,7 @@
         <v>93</v>
       </c>
       <c r="B47" s="11"/>
-      <c r="C47" s="11">
+      <c r="C47" s="38">
         <v>42</v>
       </c>
       <c r="D47" s="7">
@@ -1629,7 +1699,7 @@
         <v>94</v>
       </c>
       <c r="B48" s="11"/>
-      <c r="C48" s="11">
+      <c r="C48" s="38">
         <v>43</v>
       </c>
       <c r="D48" s="7">
@@ -1652,7 +1722,7 @@
         <v>95</v>
       </c>
       <c r="B49" s="11"/>
-      <c r="C49" s="11">
+      <c r="C49" s="38">
         <v>44</v>
       </c>
       <c r="D49" s="7">
@@ -1675,7 +1745,7 @@
         <v>96</v>
       </c>
       <c r="B50" s="11"/>
-      <c r="C50" s="11">
+      <c r="C50" s="38">
         <v>45</v>
       </c>
       <c r="D50" s="7">
@@ -1698,7 +1768,7 @@
         <v>97</v>
       </c>
       <c r="B51" s="11"/>
-      <c r="C51" s="11">
+      <c r="C51" s="38">
         <v>46</v>
       </c>
       <c r="D51" s="7">
@@ -1721,7 +1791,7 @@
         <v>98</v>
       </c>
       <c r="B52" s="11"/>
-      <c r="C52" s="11">
+      <c r="C52" s="38">
         <v>47</v>
       </c>
       <c r="D52" s="7">
@@ -1744,7 +1814,7 @@
         <v>99</v>
       </c>
       <c r="B53" s="11"/>
-      <c r="C53" s="11">
+      <c r="C53" s="38">
         <v>48</v>
       </c>
       <c r="D53" s="7">
@@ -1810,7 +1880,7 @@
       <c r="A57" s="6">
         <v>48</v>
       </c>
-      <c r="B57" s="11">
+      <c r="B57" s="38">
         <v>48</v>
       </c>
       <c r="C57" s="11"/>
@@ -1831,7 +1901,7 @@
       <c r="A58" s="6">
         <v>47</v>
       </c>
-      <c r="B58" s="11">
+      <c r="B58" s="38">
         <v>47</v>
       </c>
       <c r="C58" s="11"/>
@@ -1852,7 +1922,7 @@
       <c r="A59" s="6">
         <v>46</v>
       </c>
-      <c r="B59" s="11">
+      <c r="B59" s="38">
         <v>46</v>
       </c>
       <c r="C59" s="11"/>
@@ -1875,7 +1945,7 @@
       <c r="A60" s="6">
         <v>45</v>
       </c>
-      <c r="B60" s="11">
+      <c r="B60" s="38">
         <v>45</v>
       </c>
       <c r="C60" s="11"/>
@@ -1898,7 +1968,7 @@
       <c r="A61" s="6">
         <v>44</v>
       </c>
-      <c r="B61" s="11">
+      <c r="B61" s="38">
         <v>44</v>
       </c>
       <c r="C61" s="11"/>
@@ -1921,7 +1991,7 @@
       <c r="A62" s="6">
         <v>43</v>
       </c>
-      <c r="B62" s="11">
+      <c r="B62" s="38">
         <v>43</v>
       </c>
       <c r="C62" s="11"/>
@@ -1944,7 +2014,7 @@
       <c r="A63" s="6">
         <v>42</v>
       </c>
-      <c r="B63" s="11">
+      <c r="B63" s="38">
         <v>42</v>
       </c>
       <c r="C63" s="11"/>
@@ -1967,7 +2037,7 @@
       <c r="A64" s="6">
         <v>41</v>
       </c>
-      <c r="B64" s="11">
+      <c r="B64" s="38">
         <v>41</v>
       </c>
       <c r="C64" s="11"/>
@@ -1990,7 +2060,7 @@
       <c r="A65" s="6">
         <v>40</v>
       </c>
-      <c r="B65" s="11">
+      <c r="B65" s="38">
         <v>40</v>
       </c>
       <c r="C65" s="11"/>
@@ -2013,7 +2083,7 @@
       <c r="A66" s="6">
         <v>39</v>
       </c>
-      <c r="B66" s="11">
+      <c r="B66" s="38">
         <v>39</v>
       </c>
       <c r="C66" s="11"/>
@@ -2036,7 +2106,7 @@
       <c r="A67" s="6">
         <v>38</v>
       </c>
-      <c r="B67" s="11">
+      <c r="B67" s="38">
         <v>38</v>
       </c>
       <c r="C67" s="11"/>
@@ -2059,7 +2129,7 @@
       <c r="A68" s="6">
         <v>37</v>
       </c>
-      <c r="B68" s="11">
+      <c r="B68" s="38">
         <v>37</v>
       </c>
       <c r="C68" s="11"/>
@@ -2082,7 +2152,7 @@
       <c r="A69" s="6">
         <v>36</v>
       </c>
-      <c r="B69" s="11">
+      <c r="B69" s="38">
         <v>36</v>
       </c>
       <c r="C69" s="11"/>
@@ -2105,7 +2175,7 @@
       <c r="A70" s="6">
         <v>35</v>
       </c>
-      <c r="B70" s="11">
+      <c r="B70" s="38">
         <v>35</v>
       </c>
       <c r="C70" s="11"/>
@@ -2128,7 +2198,7 @@
       <c r="A71" s="6">
         <v>34</v>
       </c>
-      <c r="B71" s="11">
+      <c r="B71" s="38">
         <v>34</v>
       </c>
       <c r="C71" s="11"/>
@@ -2151,7 +2221,7 @@
       <c r="A72" s="6">
         <v>33</v>
       </c>
-      <c r="B72" s="11">
+      <c r="B72" s="38">
         <v>33</v>
       </c>
       <c r="C72" s="11"/>
@@ -2174,7 +2244,7 @@
       <c r="A73" s="6">
         <v>32</v>
       </c>
-      <c r="B73" s="11">
+      <c r="B73" s="38">
         <v>32</v>
       </c>
       <c r="C73" s="11"/>
@@ -2197,7 +2267,7 @@
       <c r="A74" s="6">
         <v>31</v>
       </c>
-      <c r="B74" s="11">
+      <c r="B74" s="38">
         <v>31</v>
       </c>
       <c r="C74" s="11"/>
@@ -2220,7 +2290,7 @@
       <c r="A75" s="6">
         <v>30</v>
       </c>
-      <c r="B75" s="11">
+      <c r="B75" s="38">
         <v>30</v>
       </c>
       <c r="C75" s="11"/>
@@ -2243,7 +2313,7 @@
       <c r="A76" s="6">
         <v>29</v>
       </c>
-      <c r="B76" s="11">
+      <c r="B76" s="38">
         <v>29</v>
       </c>
       <c r="C76" s="11"/>
@@ -2266,7 +2336,7 @@
       <c r="A77" s="6">
         <v>28</v>
       </c>
-      <c r="B77" s="11">
+      <c r="B77" s="38">
         <v>28</v>
       </c>
       <c r="C77" s="11"/>
@@ -2289,7 +2359,7 @@
       <c r="A78" s="6">
         <v>27</v>
       </c>
-      <c r="B78" s="11">
+      <c r="B78" s="38">
         <v>27</v>
       </c>
       <c r="C78" s="11"/>
@@ -2312,7 +2382,7 @@
       <c r="A79" s="6">
         <v>26</v>
       </c>
-      <c r="B79" s="11">
+      <c r="B79" s="38">
         <v>26</v>
       </c>
       <c r="C79" s="11"/>
@@ -2335,7 +2405,7 @@
       <c r="A80" s="6">
         <v>25</v>
       </c>
-      <c r="B80" s="11">
+      <c r="B80" s="38">
         <v>25</v>
       </c>
       <c r="C80" s="11"/>
@@ -2372,7 +2442,7 @@
       <c r="A82" s="6">
         <v>24</v>
       </c>
-      <c r="B82" s="11">
+      <c r="B82" s="38">
         <v>24</v>
       </c>
       <c r="C82" s="10"/>
@@ -2394,7 +2464,7 @@
       <c r="A83" s="6">
         <v>23</v>
       </c>
-      <c r="B83" s="11">
+      <c r="B83" s="38">
         <v>23</v>
       </c>
       <c r="C83" s="10"/>
@@ -2416,7 +2486,7 @@
       <c r="A84" s="6">
         <v>22</v>
       </c>
-      <c r="B84" s="11">
+      <c r="B84" s="38">
         <v>22</v>
       </c>
       <c r="C84" s="10"/>
@@ -2439,7 +2509,7 @@
       <c r="A85" s="6">
         <v>21</v>
       </c>
-      <c r="B85" s="11">
+      <c r="B85" s="38">
         <v>21</v>
       </c>
       <c r="C85" s="10"/>
@@ -2462,7 +2532,7 @@
       <c r="A86" s="6">
         <v>20</v>
       </c>
-      <c r="B86" s="11">
+      <c r="B86" s="38">
         <v>20</v>
       </c>
       <c r="C86" s="10"/>
@@ -2485,7 +2555,7 @@
       <c r="A87" s="6">
         <v>19</v>
       </c>
-      <c r="B87" s="11">
+      <c r="B87" s="38">
         <v>19</v>
       </c>
       <c r="C87" s="10"/>
@@ -2508,7 +2578,7 @@
       <c r="A88" s="6">
         <v>18</v>
       </c>
-      <c r="B88" s="11">
+      <c r="B88" s="38">
         <v>18</v>
       </c>
       <c r="C88" s="10"/>
@@ -2531,7 +2601,7 @@
       <c r="A89" s="6">
         <v>17</v>
       </c>
-      <c r="B89" s="11">
+      <c r="B89" s="38">
         <v>17</v>
       </c>
       <c r="C89" s="10"/>
@@ -2554,7 +2624,7 @@
       <c r="A90" s="6">
         <v>16</v>
       </c>
-      <c r="B90" s="11">
+      <c r="B90" s="38">
         <v>16</v>
       </c>
       <c r="C90" s="10"/>
@@ -2577,7 +2647,7 @@
       <c r="A91" s="6">
         <v>15</v>
       </c>
-      <c r="B91" s="11">
+      <c r="B91" s="38">
         <v>15</v>
       </c>
       <c r="C91" s="10"/>
@@ -2600,7 +2670,7 @@
       <c r="A92" s="6">
         <v>14</v>
       </c>
-      <c r="B92" s="11">
+      <c r="B92" s="38">
         <v>14</v>
       </c>
       <c r="C92" s="10"/>
@@ -2623,7 +2693,7 @@
       <c r="A93" s="6">
         <v>13</v>
       </c>
-      <c r="B93" s="11">
+      <c r="B93" s="38">
         <v>13</v>
       </c>
       <c r="C93" s="10"/>
@@ -2646,7 +2716,7 @@
       <c r="A94" s="6">
         <v>12</v>
       </c>
-      <c r="B94" s="11">
+      <c r="B94" s="38">
         <v>12</v>
       </c>
       <c r="C94" s="10"/>
@@ -2669,7 +2739,7 @@
       <c r="A95" s="6">
         <v>11</v>
       </c>
-      <c r="B95" s="11">
+      <c r="B95" s="38">
         <v>11</v>
       </c>
       <c r="C95" s="10"/>
@@ -2692,7 +2762,7 @@
       <c r="A96" s="6">
         <v>10</v>
       </c>
-      <c r="B96" s="11">
+      <c r="B96" s="38">
         <v>10</v>
       </c>
       <c r="C96" s="10"/>
@@ -2715,7 +2785,7 @@
       <c r="A97" s="6">
         <v>9</v>
       </c>
-      <c r="B97" s="11">
+      <c r="B97" s="38">
         <v>9</v>
       </c>
       <c r="C97" s="10"/>
@@ -2738,7 +2808,7 @@
       <c r="A98" s="6">
         <v>8</v>
       </c>
-      <c r="B98" s="11">
+      <c r="B98" s="38">
         <v>8</v>
       </c>
       <c r="C98" s="10"/>
@@ -2761,7 +2831,7 @@
       <c r="A99" s="6">
         <v>7</v>
       </c>
-      <c r="B99" s="11">
+      <c r="B99" s="38">
         <v>7</v>
       </c>
       <c r="C99" s="10"/>
@@ -2784,7 +2854,7 @@
       <c r="A100" s="6">
         <v>6</v>
       </c>
-      <c r="B100" s="11">
+      <c r="B100" s="38">
         <v>6</v>
       </c>
       <c r="C100" s="10"/>
@@ -2807,7 +2877,7 @@
       <c r="A101" s="6">
         <v>5</v>
       </c>
-      <c r="B101" s="11">
+      <c r="B101" s="38">
         <v>5</v>
       </c>
       <c r="C101" s="10"/>
@@ -2830,7 +2900,7 @@
       <c r="A102" s="6">
         <v>4</v>
       </c>
-      <c r="B102" s="11">
+      <c r="B102" s="38">
         <v>4</v>
       </c>
       <c r="C102" s="10"/>
@@ -2853,7 +2923,7 @@
       <c r="A103" s="6">
         <v>3</v>
       </c>
-      <c r="B103" s="11">
+      <c r="B103" s="38">
         <v>3</v>
       </c>
       <c r="C103" s="10"/>
@@ -2876,7 +2946,7 @@
       <c r="A104" s="6">
         <v>2</v>
       </c>
-      <c r="B104" s="11">
+      <c r="B104" s="38">
         <v>2</v>
       </c>
       <c r="C104" s="10"/>
@@ -2899,7 +2969,7 @@
       <c r="A105" s="6">
         <v>1</v>
       </c>
-      <c r="B105" s="11">
+      <c r="B105" s="38">
         <v>1</v>
       </c>
       <c r="C105" s="10"/>
@@ -2952,7 +3022,7 @@
       <c r="A108" s="12">
         <v>49</v>
       </c>
-      <c r="B108" s="11">
+      <c r="B108" s="38">
         <v>49</v>
       </c>
       <c r="D108" s="16"/>
@@ -2968,7 +3038,7 @@
       <c r="A109" s="12">
         <v>50</v>
       </c>
-      <c r="B109">
+      <c r="B109" s="38">
         <v>50</v>
       </c>
       <c r="D109" s="16"/>
@@ -2984,7 +3054,7 @@
       <c r="A110" s="12">
         <v>51</v>
       </c>
-      <c r="B110">
+      <c r="B110" s="38">
         <v>51</v>
       </c>
       <c r="D110" s="16"/>
@@ -3000,7 +3070,7 @@
       <c r="A111" s="12">
         <v>100</v>
       </c>
-      <c r="C111">
+      <c r="C111" s="38">
         <v>49</v>
       </c>
       <c r="D111" s="16"/>
@@ -3016,7 +3086,7 @@
       <c r="A112" s="12">
         <v>101</v>
       </c>
-      <c r="C112">
+      <c r="C112" s="38">
         <v>50</v>
       </c>
       <c r="D112" s="16"/>
@@ -3032,7 +3102,7 @@
       <c r="A113" s="13">
         <v>102</v>
       </c>
-      <c r="C113">
+      <c r="C113" s="38">
         <v>51</v>
       </c>
       <c r="D113" s="16"/>
@@ -3051,6 +3121,3172 @@
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="107" max="16383" man="1"/>
   </rowBreaks>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z117"/>
+  <sheetViews>
+    <sheetView zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V49" sqref="V49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.625" hidden="1" customWidth="1"/>
+    <col min="6" max="8" width="13" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="12" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.125" customWidth="1"/>
+    <col min="16" max="17" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="26" width="11" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>48</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="35">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1</v>
+      </c>
+      <c r="E2" s="29"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="34">
+        <v>51</v>
+      </c>
+      <c r="O2" s="40">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>47</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="35">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7">
+        <v>2</v>
+      </c>
+      <c r="E3" s="29"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="34">
+        <v>50</v>
+      </c>
+      <c r="O3" s="40">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>46</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="35">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7">
+        <f>D3+1</f>
+        <v>3</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="34">
+        <v>49</v>
+      </c>
+      <c r="O4" s="40">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>45</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="35">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" ref="D5:D69" si="0">D4+1</f>
+        <v>4</v>
+      </c>
+      <c r="E5" s="29"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="34">
+        <v>48</v>
+      </c>
+      <c r="O5" s="40">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>44</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="35">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E6" s="29"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="34">
+        <v>47</v>
+      </c>
+      <c r="O6" s="40">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>43</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="35">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="34">
+        <v>46</v>
+      </c>
+      <c r="O7" s="40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>42</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="35">
+        <v>7</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E8" s="29"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="34">
+        <v>45</v>
+      </c>
+      <c r="O8" s="40">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>41</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="35">
+        <v>8</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E9" s="29"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="34">
+        <v>44</v>
+      </c>
+      <c r="O9" s="40">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>40</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="35">
+        <v>9</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E10" s="29"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="34">
+        <v>43</v>
+      </c>
+      <c r="O10" s="40">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>39</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="35">
+        <v>10</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E11" s="29"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="34">
+        <v>42</v>
+      </c>
+      <c r="O11" s="40">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>38</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="35">
+        <v>11</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E12" s="29"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="34">
+        <v>41</v>
+      </c>
+      <c r="O12" s="40">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>37</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="35">
+        <v>12</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E13" s="29"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="34">
+        <v>40</v>
+      </c>
+      <c r="O13" s="40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>36</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="35">
+        <v>13</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E14" s="29"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="34">
+        <v>39</v>
+      </c>
+      <c r="O14" s="40">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>35</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="35">
+        <v>14</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E15" s="29"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="34">
+        <v>38</v>
+      </c>
+      <c r="O15" s="40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>34</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="35">
+        <v>15</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E16" s="29"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="34">
+        <v>37</v>
+      </c>
+      <c r="O16" s="40">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>33</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="35">
+        <v>16</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E17" s="29"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="34">
+        <v>36</v>
+      </c>
+      <c r="O17" s="40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="30"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="36">
+        <v>35</v>
+      </c>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>32</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="35">
+        <v>17</v>
+      </c>
+      <c r="D19" s="7">
+        <f>D17+1</f>
+        <v>17</v>
+      </c>
+      <c r="E19" s="29"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="34">
+        <v>34</v>
+      </c>
+      <c r="O19" s="40">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>31</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="35">
+        <v>18</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E20" s="29"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="34">
+        <v>33</v>
+      </c>
+      <c r="O20" s="40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>30</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="35">
+        <v>19</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="E21" s="29"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="34">
+        <v>32</v>
+      </c>
+      <c r="O21" s="40">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>29</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="35">
+        <v>20</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E22" s="29"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="34">
+        <v>31</v>
+      </c>
+      <c r="O22" s="40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>28</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="35">
+        <v>21</v>
+      </c>
+      <c r="D23" s="7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="E23" s="29"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="34">
+        <v>30</v>
+      </c>
+      <c r="O23" s="40">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>27</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="35">
+        <v>22</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="E24" s="29"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="34">
+        <v>29</v>
+      </c>
+      <c r="O24" s="40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>26</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="35">
+        <v>23</v>
+      </c>
+      <c r="D25" s="7">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="E25" s="29"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="34">
+        <v>28</v>
+      </c>
+      <c r="O25" s="40">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>25</v>
+      </c>
+      <c r="B26" s="10"/>
+      <c r="C26" s="35">
+        <v>24</v>
+      </c>
+      <c r="D26" s="7">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="E26" s="29"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="34">
+        <v>27</v>
+      </c>
+      <c r="O26" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="36">
+        <v>13</v>
+      </c>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="37">
+        <f>D26+1</f>
+        <v>25</v>
+      </c>
+      <c r="E28" s="29"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="37">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>24</v>
+      </c>
+      <c r="B30" s="11"/>
+      <c r="C30" s="35">
+        <v>25</v>
+      </c>
+      <c r="D30" s="7">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="34">
+        <v>26</v>
+      </c>
+      <c r="N30" s="40">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>23</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="35">
+        <v>26</v>
+      </c>
+      <c r="D31" s="7">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="E31" s="11"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="34">
+        <v>25</v>
+      </c>
+      <c r="N31" s="40">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>22</v>
+      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="35">
+        <v>27</v>
+      </c>
+      <c r="D32" s="7">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="34">
+        <v>24</v>
+      </c>
+      <c r="N32" s="40">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>21</v>
+      </c>
+      <c r="B33" s="11"/>
+      <c r="C33" s="35">
+        <v>28</v>
+      </c>
+      <c r="D33" s="7">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E33" s="11"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="34">
+        <v>23</v>
+      </c>
+      <c r="N33" s="40">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>20</v>
+      </c>
+      <c r="B34" s="11"/>
+      <c r="C34" s="35">
+        <v>29</v>
+      </c>
+      <c r="D34" s="7">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="34">
+        <v>22</v>
+      </c>
+      <c r="N34" s="40">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>19</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="35">
+        <v>30</v>
+      </c>
+      <c r="D35" s="7">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="34">
+        <v>21</v>
+      </c>
+      <c r="N35" s="40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>18</v>
+      </c>
+      <c r="B36" s="11"/>
+      <c r="C36" s="35">
+        <v>31</v>
+      </c>
+      <c r="D36" s="7">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="E36" s="11"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="34">
+        <v>20</v>
+      </c>
+      <c r="N36" s="40">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <v>17</v>
+      </c>
+      <c r="B37" s="11"/>
+      <c r="C37" s="35">
+        <v>32</v>
+      </c>
+      <c r="D37" s="7">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="34">
+        <v>19</v>
+      </c>
+      <c r="N37" s="40">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" s="17"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="36">
+        <v>18</v>
+      </c>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" s="17"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="36">
+        <v>17</v>
+      </c>
+      <c r="M39" s="16"/>
+      <c r="N39" s="16"/>
+      <c r="O39" s="16"/>
+      <c r="P39" s="16"/>
+      <c r="Q39" s="16"/>
+      <c r="R39" s="16"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
+        <v>16</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="35">
+        <v>33</v>
+      </c>
+      <c r="D40" s="7">
+        <f>D37+1</f>
+        <v>35</v>
+      </c>
+      <c r="E40" s="11"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="34">
+        <v>16</v>
+      </c>
+      <c r="N40" s="40">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <v>15</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="35">
+        <v>34</v>
+      </c>
+      <c r="D41" s="7">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E41" s="11"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="34">
+        <v>15</v>
+      </c>
+      <c r="N41" s="40">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>14</v>
+      </c>
+      <c r="B42" s="11"/>
+      <c r="C42" s="35">
+        <v>35</v>
+      </c>
+      <c r="D42" s="7">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="E42" s="11"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="34">
+        <v>14</v>
+      </c>
+      <c r="N42" s="40">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>13</v>
+      </c>
+      <c r="B43" s="11"/>
+      <c r="C43" s="35">
+        <v>36</v>
+      </c>
+      <c r="D43" s="7">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="E43" s="11"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="34">
+        <v>13</v>
+      </c>
+      <c r="N43" s="40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>12</v>
+      </c>
+      <c r="B44" s="11"/>
+      <c r="C44" s="35">
+        <v>37</v>
+      </c>
+      <c r="D44" s="7">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="E44" s="11"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="34">
+        <v>12</v>
+      </c>
+      <c r="N44" s="40">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>11</v>
+      </c>
+      <c r="B45" s="11"/>
+      <c r="C45" s="35">
+        <v>38</v>
+      </c>
+      <c r="D45" s="7">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E45" s="11"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="29"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="34">
+        <v>11</v>
+      </c>
+      <c r="N45" s="40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>10</v>
+      </c>
+      <c r="B46" s="11"/>
+      <c r="C46" s="35">
+        <v>39</v>
+      </c>
+      <c r="D46" s="7">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="E46" s="11"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="29"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="34">
+        <v>10</v>
+      </c>
+      <c r="N46" s="40">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>9</v>
+      </c>
+      <c r="B47" s="11"/>
+      <c r="C47" s="35">
+        <v>40</v>
+      </c>
+      <c r="D47" s="7">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E47" s="11"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="29"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="34">
+        <v>9</v>
+      </c>
+      <c r="N47" s="40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>8</v>
+      </c>
+      <c r="B48" s="11"/>
+      <c r="C48" s="35">
+        <v>41</v>
+      </c>
+      <c r="D48" s="7">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="E48" s="11"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="29"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="34">
+        <v>8</v>
+      </c>
+      <c r="N48" s="40">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>7</v>
+      </c>
+      <c r="B49" s="11"/>
+      <c r="C49" s="35">
+        <v>42</v>
+      </c>
+      <c r="D49" s="7">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="E49" s="11"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="29"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="34">
+        <v>7</v>
+      </c>
+      <c r="N49" s="40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>6</v>
+      </c>
+      <c r="B50" s="11"/>
+      <c r="C50" s="35">
+        <v>43</v>
+      </c>
+      <c r="D50" s="7">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="E50" s="11"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="29"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="34">
+        <v>6</v>
+      </c>
+      <c r="N50" s="40">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>5</v>
+      </c>
+      <c r="B51" s="11"/>
+      <c r="C51" s="35">
+        <v>44</v>
+      </c>
+      <c r="D51" s="7">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="E51" s="11"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="29"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="34">
+        <v>5</v>
+      </c>
+      <c r="N51" s="40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>4</v>
+      </c>
+      <c r="B52" s="11"/>
+      <c r="C52" s="35">
+        <v>45</v>
+      </c>
+      <c r="D52" s="7">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="E52" s="11"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="29"/>
+      <c r="K52" s="11"/>
+      <c r="L52" s="34">
+        <v>4</v>
+      </c>
+      <c r="N52" s="40">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
+        <v>3</v>
+      </c>
+      <c r="B53" s="11"/>
+      <c r="C53" s="35">
+        <v>46</v>
+      </c>
+      <c r="D53" s="7">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="E53" s="11"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="29"/>
+      <c r="K53" s="11"/>
+      <c r="L53" s="34">
+        <v>3</v>
+      </c>
+      <c r="N53" s="40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>2</v>
+      </c>
+      <c r="B54" s="11"/>
+      <c r="C54" s="35">
+        <v>47</v>
+      </c>
+      <c r="D54" s="7">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="E54" s="11"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="29"/>
+      <c r="K54" s="11"/>
+      <c r="L54" s="34">
+        <v>2</v>
+      </c>
+      <c r="N54" s="40">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>1</v>
+      </c>
+      <c r="B55" s="11"/>
+      <c r="C55" s="35">
+        <v>48</v>
+      </c>
+      <c r="D55" s="7">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E55" s="11"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="29"/>
+      <c r="K55" s="11"/>
+      <c r="L55" s="34">
+        <v>1</v>
+      </c>
+      <c r="N55" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A56" s="17"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="19"/>
+      <c r="K56" s="16"/>
+      <c r="L56" s="16"/>
+      <c r="M56" s="16"/>
+      <c r="N56" s="36">
+        <v>13</v>
+      </c>
+      <c r="O56" s="16"/>
+      <c r="P56" s="16"/>
+      <c r="Q56" s="16"/>
+      <c r="R56" s="16"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57" s="16"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="37">
+        <f>D55+1</f>
+        <v>51</v>
+      </c>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="16"/>
+      <c r="M57" s="16"/>
+      <c r="N57" s="16"/>
+      <c r="O57" s="16"/>
+      <c r="P57" s="16"/>
+      <c r="Q57" s="16"/>
+      <c r="R57" s="16"/>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>99</v>
+      </c>
+      <c r="B58" s="35">
+        <v>48</v>
+      </c>
+      <c r="C58" s="11"/>
+      <c r="D58" s="7">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="29"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="29"/>
+      <c r="M58" s="34">
+        <v>1</v>
+      </c>
+      <c r="P58" s="40">
+        <v>1</v>
+      </c>
+      <c r="R58" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>98</v>
+      </c>
+      <c r="B59" s="35">
+        <v>47</v>
+      </c>
+      <c r="C59" s="11"/>
+      <c r="D59" s="7">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="29"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="11"/>
+      <c r="J59" s="11"/>
+      <c r="K59" s="29"/>
+      <c r="M59" s="34">
+        <v>2</v>
+      </c>
+      <c r="P59" s="40">
+        <v>14</v>
+      </c>
+      <c r="R59" s="39">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A60" s="6">
+        <v>97</v>
+      </c>
+      <c r="B60" s="35">
+        <v>46</v>
+      </c>
+      <c r="C60" s="11"/>
+      <c r="D60" s="7">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="29"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="29"/>
+      <c r="M60" s="34">
+        <v>3</v>
+      </c>
+      <c r="P60" s="40">
+        <v>2</v>
+      </c>
+      <c r="R60" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A61" s="6">
+        <v>96</v>
+      </c>
+      <c r="B61" s="35">
+        <v>45</v>
+      </c>
+      <c r="C61" s="11"/>
+      <c r="D61" s="7">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="29"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="11"/>
+      <c r="J61" s="11"/>
+      <c r="K61" s="29"/>
+      <c r="M61" s="34">
+        <v>4</v>
+      </c>
+      <c r="P61" s="40">
+        <v>15</v>
+      </c>
+      <c r="R61" s="39">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A62" s="6">
+        <v>95</v>
+      </c>
+      <c r="B62" s="35">
+        <v>44</v>
+      </c>
+      <c r="C62" s="11"/>
+      <c r="D62" s="7">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="29"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="11"/>
+      <c r="J62" s="11"/>
+      <c r="K62" s="29"/>
+      <c r="M62" s="34">
+        <v>5</v>
+      </c>
+      <c r="P62" s="40">
+        <v>3</v>
+      </c>
+      <c r="R62" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A63" s="6">
+        <v>94</v>
+      </c>
+      <c r="B63" s="35">
+        <v>43</v>
+      </c>
+      <c r="C63" s="11"/>
+      <c r="D63" s="7">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="29"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="11"/>
+      <c r="J63" s="11"/>
+      <c r="K63" s="29"/>
+      <c r="M63" s="34">
+        <v>6</v>
+      </c>
+      <c r="P63" s="40">
+        <v>16</v>
+      </c>
+      <c r="R63" s="39">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A64" s="6">
+        <v>93</v>
+      </c>
+      <c r="B64" s="35">
+        <v>42</v>
+      </c>
+      <c r="C64" s="11"/>
+      <c r="D64" s="7">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="29"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="29"/>
+      <c r="M64" s="34">
+        <v>7</v>
+      </c>
+      <c r="P64" s="40">
+        <v>4</v>
+      </c>
+      <c r="R64" s="39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A65" s="6">
+        <v>92</v>
+      </c>
+      <c r="B65" s="35">
+        <v>41</v>
+      </c>
+      <c r="C65" s="11"/>
+      <c r="D65" s="7">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="29"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="11"/>
+      <c r="J65" s="11"/>
+      <c r="K65" s="29"/>
+      <c r="M65" s="34">
+        <v>8</v>
+      </c>
+      <c r="P65" s="40">
+        <v>17</v>
+      </c>
+      <c r="R65" s="39">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A66" s="6">
+        <v>91</v>
+      </c>
+      <c r="B66" s="35">
+        <v>40</v>
+      </c>
+      <c r="C66" s="11"/>
+      <c r="D66" s="7">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="29"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="11"/>
+      <c r="J66" s="11"/>
+      <c r="K66" s="29"/>
+      <c r="M66" s="34">
+        <v>9</v>
+      </c>
+      <c r="P66" s="40">
+        <v>5</v>
+      </c>
+      <c r="R66" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A67" s="6">
+        <v>90</v>
+      </c>
+      <c r="B67" s="35">
+        <v>39</v>
+      </c>
+      <c r="C67" s="11"/>
+      <c r="D67" s="7">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="29"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="11"/>
+      <c r="J67" s="11"/>
+      <c r="K67" s="29"/>
+      <c r="M67" s="34">
+        <v>10</v>
+      </c>
+      <c r="P67" s="40">
+        <v>18</v>
+      </c>
+      <c r="R67" s="39">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A68" s="6">
+        <v>89</v>
+      </c>
+      <c r="B68" s="35">
+        <v>38</v>
+      </c>
+      <c r="C68" s="11"/>
+      <c r="D68" s="7">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="29"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="11"/>
+      <c r="J68" s="11"/>
+      <c r="K68" s="29"/>
+      <c r="M68" s="34">
+        <v>11</v>
+      </c>
+      <c r="P68" s="40">
+        <v>6</v>
+      </c>
+      <c r="R68" s="39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A69" s="6">
+        <v>88</v>
+      </c>
+      <c r="B69" s="35">
+        <v>37</v>
+      </c>
+      <c r="C69" s="11"/>
+      <c r="D69" s="7">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="29"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="11"/>
+      <c r="J69" s="11"/>
+      <c r="K69" s="29"/>
+      <c r="M69" s="34">
+        <v>12</v>
+      </c>
+      <c r="P69" s="40">
+        <v>19</v>
+      </c>
+      <c r="R69" s="39">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A70" s="6">
+        <v>87</v>
+      </c>
+      <c r="B70" s="35">
+        <v>36</v>
+      </c>
+      <c r="C70" s="11"/>
+      <c r="D70" s="7">
+        <f t="shared" ref="D70:D108" si="1">D69+1</f>
+        <v>64</v>
+      </c>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="29"/>
+      <c r="H70" s="11"/>
+      <c r="I70" s="11"/>
+      <c r="J70" s="11"/>
+      <c r="K70" s="29"/>
+      <c r="M70" s="34">
+        <v>13</v>
+      </c>
+      <c r="P70" s="40">
+        <v>7</v>
+      </c>
+      <c r="R70" s="39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A71" s="6">
+        <v>86</v>
+      </c>
+      <c r="B71" s="35">
+        <v>35</v>
+      </c>
+      <c r="C71" s="11"/>
+      <c r="D71" s="7">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="29"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="11"/>
+      <c r="K71" s="29"/>
+      <c r="M71" s="34">
+        <v>14</v>
+      </c>
+      <c r="P71" s="40">
+        <v>20</v>
+      </c>
+      <c r="R71" s="39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A72" s="6">
+        <v>85</v>
+      </c>
+      <c r="B72" s="35">
+        <v>34</v>
+      </c>
+      <c r="C72" s="11"/>
+      <c r="D72" s="7">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="29"/>
+      <c r="H72" s="11"/>
+      <c r="I72" s="11"/>
+      <c r="J72" s="11"/>
+      <c r="K72" s="29"/>
+      <c r="M72" s="34">
+        <v>15</v>
+      </c>
+      <c r="P72" s="40">
+        <v>8</v>
+      </c>
+      <c r="R72" s="39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A73" s="6">
+        <v>84</v>
+      </c>
+      <c r="B73" s="35">
+        <v>33</v>
+      </c>
+      <c r="C73" s="11"/>
+      <c r="D73" s="7">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="29"/>
+      <c r="H73" s="11"/>
+      <c r="I73" s="11"/>
+      <c r="J73" s="11"/>
+      <c r="K73" s="29"/>
+      <c r="M73" s="34">
+        <v>16</v>
+      </c>
+      <c r="P73" s="40">
+        <v>21</v>
+      </c>
+      <c r="R73" s="39">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A74" s="16"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="19"/>
+      <c r="H74" s="16"/>
+      <c r="I74" s="16"/>
+      <c r="J74" s="16"/>
+      <c r="K74" s="19"/>
+      <c r="L74" s="16"/>
+      <c r="M74" s="36">
+        <v>17</v>
+      </c>
+      <c r="N74" s="16"/>
+      <c r="O74" s="16"/>
+      <c r="P74" s="16"/>
+      <c r="Q74" s="16"/>
+      <c r="R74" s="16"/>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A75" s="16"/>
+      <c r="B75" s="16"/>
+      <c r="C75" s="16"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="16"/>
+      <c r="F75" s="16"/>
+      <c r="G75" s="19"/>
+      <c r="H75" s="16"/>
+      <c r="I75" s="16"/>
+      <c r="J75" s="16"/>
+      <c r="K75" s="19"/>
+      <c r="L75" s="16"/>
+      <c r="M75" s="36">
+        <v>18</v>
+      </c>
+      <c r="N75" s="16"/>
+      <c r="O75" s="16"/>
+      <c r="P75" s="16"/>
+      <c r="Q75" s="16"/>
+      <c r="R75" s="16"/>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A76" s="6">
+        <v>83</v>
+      </c>
+      <c r="B76" s="35">
+        <v>32</v>
+      </c>
+      <c r="C76" s="11"/>
+      <c r="D76" s="7">
+        <f>D73+1</f>
+        <v>68</v>
+      </c>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="29"/>
+      <c r="H76" s="11"/>
+      <c r="I76" s="11"/>
+      <c r="J76" s="11"/>
+      <c r="K76" s="29"/>
+      <c r="M76" s="34">
+        <v>19</v>
+      </c>
+      <c r="P76" s="40">
+        <v>9</v>
+      </c>
+      <c r="R76" s="39">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A77" s="6">
+        <v>82</v>
+      </c>
+      <c r="B77" s="35">
+        <v>31</v>
+      </c>
+      <c r="C77" s="11"/>
+      <c r="D77" s="7">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="29"/>
+      <c r="H77" s="11"/>
+      <c r="I77" s="11"/>
+      <c r="J77" s="11"/>
+      <c r="K77" s="29"/>
+      <c r="M77" s="34">
+        <v>20</v>
+      </c>
+      <c r="P77" s="40">
+        <v>22</v>
+      </c>
+      <c r="R77" s="39">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A78" s="6">
+        <v>81</v>
+      </c>
+      <c r="B78" s="35">
+        <v>30</v>
+      </c>
+      <c r="C78" s="11"/>
+      <c r="D78" s="7">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="29"/>
+      <c r="H78" s="11"/>
+      <c r="I78" s="11"/>
+      <c r="J78" s="11"/>
+      <c r="K78" s="29"/>
+      <c r="M78" s="34">
+        <v>21</v>
+      </c>
+      <c r="P78" s="40">
+        <v>10</v>
+      </c>
+      <c r="R78" s="39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A79" s="6">
+        <v>80</v>
+      </c>
+      <c r="B79" s="35">
+        <v>29</v>
+      </c>
+      <c r="C79" s="11"/>
+      <c r="D79" s="7">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="29"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="11"/>
+      <c r="J79" s="11"/>
+      <c r="K79" s="29"/>
+      <c r="M79" s="34">
+        <v>22</v>
+      </c>
+      <c r="P79" s="40">
+        <v>23</v>
+      </c>
+      <c r="R79" s="39">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A80" s="6">
+        <v>79</v>
+      </c>
+      <c r="B80" s="35">
+        <v>28</v>
+      </c>
+      <c r="C80" s="11"/>
+      <c r="D80" s="7">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="29"/>
+      <c r="H80" s="11"/>
+      <c r="I80" s="11"/>
+      <c r="J80" s="11"/>
+      <c r="K80" s="29"/>
+      <c r="M80" s="34">
+        <v>23</v>
+      </c>
+      <c r="P80" s="40">
+        <v>11</v>
+      </c>
+      <c r="R80" s="39">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A81" s="6">
+        <v>78</v>
+      </c>
+      <c r="B81" s="35">
+        <v>27</v>
+      </c>
+      <c r="C81" s="11"/>
+      <c r="D81" s="7">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="E81" s="11"/>
+      <c r="F81" s="11"/>
+      <c r="G81" s="29"/>
+      <c r="H81" s="11"/>
+      <c r="I81" s="11"/>
+      <c r="J81" s="11"/>
+      <c r="K81" s="29"/>
+      <c r="M81" s="34">
+        <v>24</v>
+      </c>
+      <c r="P81" s="40">
+        <v>24</v>
+      </c>
+      <c r="R81" s="39">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A82" s="6">
+        <v>77</v>
+      </c>
+      <c r="B82" s="35">
+        <v>26</v>
+      </c>
+      <c r="C82" s="11"/>
+      <c r="D82" s="7">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="E82" s="11"/>
+      <c r="F82" s="11"/>
+      <c r="G82" s="29"/>
+      <c r="H82" s="11"/>
+      <c r="I82" s="11"/>
+      <c r="J82" s="11"/>
+      <c r="K82" s="29"/>
+      <c r="M82" s="34">
+        <v>25</v>
+      </c>
+      <c r="P82" s="40">
+        <v>12</v>
+      </c>
+      <c r="R82" s="39">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A83" s="6">
+        <v>76</v>
+      </c>
+      <c r="B83" s="35">
+        <v>25</v>
+      </c>
+      <c r="C83" s="11"/>
+      <c r="D83" s="7">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="29"/>
+      <c r="H83" s="11"/>
+      <c r="I83" s="11"/>
+      <c r="J83" s="11"/>
+      <c r="K83" s="29"/>
+      <c r="M83" s="34">
+        <v>26</v>
+      </c>
+      <c r="P83" s="40">
+        <v>25</v>
+      </c>
+      <c r="R83" s="39">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A84" s="16"/>
+      <c r="B84" s="16"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="16"/>
+      <c r="F84" s="16"/>
+      <c r="G84" s="19"/>
+      <c r="H84" s="16"/>
+      <c r="I84" s="16"/>
+      <c r="J84" s="16"/>
+      <c r="K84" s="19"/>
+      <c r="L84" s="16"/>
+      <c r="M84" s="16"/>
+      <c r="N84" s="16"/>
+      <c r="O84" s="16"/>
+      <c r="P84" s="36">
+        <v>13</v>
+      </c>
+      <c r="Q84" s="16"/>
+      <c r="R84" s="16"/>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A85" s="6">
+        <v>75</v>
+      </c>
+      <c r="B85" s="35">
+        <v>24</v>
+      </c>
+      <c r="C85" s="10"/>
+      <c r="D85" s="7">
+        <f>D83+1</f>
+        <v>76</v>
+      </c>
+      <c r="E85" s="11"/>
+      <c r="F85" s="11"/>
+      <c r="G85" s="11"/>
+      <c r="H85" s="29"/>
+      <c r="I85" s="11"/>
+      <c r="J85" s="14"/>
+      <c r="K85" s="15"/>
+      <c r="M85" s="34">
+        <v>27</v>
+      </c>
+      <c r="Q85" s="40">
+        <v>1</v>
+      </c>
+      <c r="R85" s="39">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A86" s="6">
+        <v>74</v>
+      </c>
+      <c r="B86" s="35">
+        <v>23</v>
+      </c>
+      <c r="C86" s="10"/>
+      <c r="D86" s="7">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="E86" s="11"/>
+      <c r="F86" s="11"/>
+      <c r="G86" s="11"/>
+      <c r="H86" s="29"/>
+      <c r="I86" s="11"/>
+      <c r="J86" s="14"/>
+      <c r="K86" s="15"/>
+      <c r="M86" s="34">
+        <v>28</v>
+      </c>
+      <c r="Q86" s="40">
+        <v>14</v>
+      </c>
+      <c r="R86" s="39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A87" s="6">
+        <v>73</v>
+      </c>
+      <c r="B87" s="35">
+        <v>22</v>
+      </c>
+      <c r="C87" s="10"/>
+      <c r="D87" s="7">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="E87" s="11"/>
+      <c r="F87" s="11"/>
+      <c r="G87" s="11"/>
+      <c r="H87" s="29"/>
+      <c r="I87" s="11"/>
+      <c r="J87" s="14"/>
+      <c r="K87" s="15"/>
+      <c r="M87" s="34">
+        <v>29</v>
+      </c>
+      <c r="Q87" s="40">
+        <v>2</v>
+      </c>
+      <c r="R87" s="39">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A88" s="6">
+        <v>72</v>
+      </c>
+      <c r="B88" s="35">
+        <v>21</v>
+      </c>
+      <c r="C88" s="10"/>
+      <c r="D88" s="7">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="E88" s="11"/>
+      <c r="F88" s="11"/>
+      <c r="G88" s="11"/>
+      <c r="H88" s="29"/>
+      <c r="I88" s="11"/>
+      <c r="J88" s="14"/>
+      <c r="K88" s="15"/>
+      <c r="M88" s="34">
+        <v>30</v>
+      </c>
+      <c r="Q88" s="40">
+        <v>15</v>
+      </c>
+      <c r="R88" s="39">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A89" s="6">
+        <v>71</v>
+      </c>
+      <c r="B89" s="35">
+        <v>20</v>
+      </c>
+      <c r="C89" s="10"/>
+      <c r="D89" s="7">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="E89" s="11"/>
+      <c r="F89" s="11"/>
+      <c r="G89" s="11"/>
+      <c r="H89" s="29"/>
+      <c r="I89" s="11"/>
+      <c r="J89" s="14"/>
+      <c r="K89" s="15"/>
+      <c r="M89" s="34">
+        <v>31</v>
+      </c>
+      <c r="Q89" s="40">
+        <v>3</v>
+      </c>
+      <c r="R89" s="39">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A90" s="6">
+        <v>70</v>
+      </c>
+      <c r="B90" s="35">
+        <v>19</v>
+      </c>
+      <c r="C90" s="10"/>
+      <c r="D90" s="7">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="E90" s="11"/>
+      <c r="F90" s="11"/>
+      <c r="G90" s="11"/>
+      <c r="H90" s="29"/>
+      <c r="I90" s="11"/>
+      <c r="J90" s="14"/>
+      <c r="K90" s="15"/>
+      <c r="M90" s="34">
+        <v>32</v>
+      </c>
+      <c r="Q90" s="40">
+        <v>16</v>
+      </c>
+      <c r="R90" s="39">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A91" s="6">
+        <v>69</v>
+      </c>
+      <c r="B91" s="35">
+        <v>18</v>
+      </c>
+      <c r="C91" s="10"/>
+      <c r="D91" s="7">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="E91" s="11"/>
+      <c r="F91" s="11"/>
+      <c r="G91" s="11"/>
+      <c r="H91" s="29"/>
+      <c r="I91" s="11"/>
+      <c r="J91" s="14"/>
+      <c r="K91" s="15"/>
+      <c r="M91" s="34">
+        <v>33</v>
+      </c>
+      <c r="Q91" s="40">
+        <v>4</v>
+      </c>
+      <c r="R91" s="39">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A92" s="6">
+        <v>68</v>
+      </c>
+      <c r="B92" s="35">
+        <v>17</v>
+      </c>
+      <c r="C92" s="10"/>
+      <c r="D92" s="7">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="E92" s="11"/>
+      <c r="F92" s="11"/>
+      <c r="G92" s="11"/>
+      <c r="H92" s="29"/>
+      <c r="I92" s="11"/>
+      <c r="J92" s="14"/>
+      <c r="K92" s="15"/>
+      <c r="M92" s="34">
+        <v>34</v>
+      </c>
+      <c r="Q92" s="40">
+        <v>17</v>
+      </c>
+      <c r="R92" s="39">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A93" s="16"/>
+      <c r="B93" s="16"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="20"/>
+      <c r="E93" s="16"/>
+      <c r="F93" s="16"/>
+      <c r="G93" s="16"/>
+      <c r="H93" s="19"/>
+      <c r="I93" s="16"/>
+      <c r="J93" s="21"/>
+      <c r="K93" s="22"/>
+      <c r="L93" s="16"/>
+      <c r="M93" s="36">
+        <v>35</v>
+      </c>
+      <c r="N93" s="16"/>
+      <c r="O93" s="16"/>
+      <c r="P93" s="16"/>
+      <c r="Q93" s="16"/>
+      <c r="R93" s="16"/>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A94" s="6">
+        <v>67</v>
+      </c>
+      <c r="B94" s="35">
+        <v>16</v>
+      </c>
+      <c r="C94" s="10"/>
+      <c r="D94" s="7">
+        <f>D92+1</f>
+        <v>84</v>
+      </c>
+      <c r="E94" s="11"/>
+      <c r="F94" s="11"/>
+      <c r="G94" s="11"/>
+      <c r="H94" s="29"/>
+      <c r="I94" s="11"/>
+      <c r="J94" s="14"/>
+      <c r="K94" s="15"/>
+      <c r="M94" s="34">
+        <v>36</v>
+      </c>
+      <c r="Q94" s="40">
+        <v>5</v>
+      </c>
+      <c r="R94" s="39">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A95" s="6">
+        <v>66</v>
+      </c>
+      <c r="B95" s="35">
+        <v>15</v>
+      </c>
+      <c r="C95" s="10"/>
+      <c r="D95" s="7">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="E95" s="11"/>
+      <c r="F95" s="11"/>
+      <c r="G95" s="11"/>
+      <c r="H95" s="29"/>
+      <c r="I95" s="11"/>
+      <c r="J95" s="14"/>
+      <c r="K95" s="15"/>
+      <c r="M95" s="34">
+        <v>37</v>
+      </c>
+      <c r="Q95" s="40">
+        <v>18</v>
+      </c>
+      <c r="R95" s="39">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A96" s="6">
+        <v>65</v>
+      </c>
+      <c r="B96" s="35">
+        <v>14</v>
+      </c>
+      <c r="C96" s="10"/>
+      <c r="D96" s="7">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="E96" s="11"/>
+      <c r="F96" s="11"/>
+      <c r="G96" s="11"/>
+      <c r="H96" s="29"/>
+      <c r="I96" s="11"/>
+      <c r="J96" s="14"/>
+      <c r="K96" s="15"/>
+      <c r="M96" s="34">
+        <v>38</v>
+      </c>
+      <c r="Q96" s="40">
+        <v>6</v>
+      </c>
+      <c r="R96" s="39">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A97" s="6">
+        <v>64</v>
+      </c>
+      <c r="B97" s="35">
+        <v>13</v>
+      </c>
+      <c r="C97" s="10"/>
+      <c r="D97" s="7">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="E97" s="11"/>
+      <c r="F97" s="11"/>
+      <c r="G97" s="11"/>
+      <c r="H97" s="29"/>
+      <c r="I97" s="11"/>
+      <c r="J97" s="14"/>
+      <c r="K97" s="15"/>
+      <c r="M97" s="34">
+        <v>39</v>
+      </c>
+      <c r="Q97" s="40">
+        <v>19</v>
+      </c>
+      <c r="R97" s="39">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A98" s="6">
+        <v>63</v>
+      </c>
+      <c r="B98" s="35">
+        <v>12</v>
+      </c>
+      <c r="C98" s="10"/>
+      <c r="D98" s="7">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="E98" s="11"/>
+      <c r="F98" s="11"/>
+      <c r="G98" s="11"/>
+      <c r="H98" s="29"/>
+      <c r="I98" s="11"/>
+      <c r="J98" s="14"/>
+      <c r="K98" s="15"/>
+      <c r="M98" s="34">
+        <v>40</v>
+      </c>
+      <c r="Q98" s="40">
+        <v>7</v>
+      </c>
+      <c r="R98" s="39">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A99" s="6">
+        <v>62</v>
+      </c>
+      <c r="B99" s="35">
+        <v>11</v>
+      </c>
+      <c r="C99" s="10"/>
+      <c r="D99" s="7">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="E99" s="11"/>
+      <c r="F99" s="11"/>
+      <c r="G99" s="11"/>
+      <c r="H99" s="29"/>
+      <c r="I99" s="11"/>
+      <c r="J99" s="14"/>
+      <c r="K99" s="15"/>
+      <c r="M99" s="34">
+        <v>41</v>
+      </c>
+      <c r="Q99" s="40">
+        <v>20</v>
+      </c>
+      <c r="R99" s="39">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A100" s="6">
+        <v>61</v>
+      </c>
+      <c r="B100" s="35">
+        <v>10</v>
+      </c>
+      <c r="C100" s="10"/>
+      <c r="D100" s="7">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="E100" s="11"/>
+      <c r="F100" s="11"/>
+      <c r="G100" s="11"/>
+      <c r="H100" s="29"/>
+      <c r="I100" s="11"/>
+      <c r="J100" s="14"/>
+      <c r="K100" s="15"/>
+      <c r="M100" s="34">
+        <v>42</v>
+      </c>
+      <c r="Q100" s="40">
+        <v>8</v>
+      </c>
+      <c r="R100" s="39">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A101" s="6">
+        <v>60</v>
+      </c>
+      <c r="B101" s="35">
+        <v>9</v>
+      </c>
+      <c r="C101" s="10"/>
+      <c r="D101" s="7">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="E101" s="11"/>
+      <c r="F101" s="11"/>
+      <c r="G101" s="11"/>
+      <c r="H101" s="29"/>
+      <c r="I101" s="11"/>
+      <c r="J101" s="14"/>
+      <c r="K101" s="15"/>
+      <c r="M101" s="34">
+        <v>43</v>
+      </c>
+      <c r="Q101" s="40">
+        <v>21</v>
+      </c>
+      <c r="R101" s="39">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A102" s="6">
+        <v>59</v>
+      </c>
+      <c r="B102" s="35">
+        <v>8</v>
+      </c>
+      <c r="C102" s="10"/>
+      <c r="D102" s="7">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="E102" s="11"/>
+      <c r="F102" s="11"/>
+      <c r="G102" s="11"/>
+      <c r="H102" s="29"/>
+      <c r="I102" s="11"/>
+      <c r="J102" s="14"/>
+      <c r="K102" s="15"/>
+      <c r="M102" s="34">
+        <v>44</v>
+      </c>
+      <c r="Q102" s="40">
+        <v>9</v>
+      </c>
+      <c r="R102" s="39">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A103" s="6">
+        <v>58</v>
+      </c>
+      <c r="B103" s="35">
+        <v>7</v>
+      </c>
+      <c r="C103" s="10"/>
+      <c r="D103" s="7">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="E103" s="11"/>
+      <c r="F103" s="11"/>
+      <c r="G103" s="11"/>
+      <c r="H103" s="29"/>
+      <c r="I103" s="11"/>
+      <c r="J103" s="14"/>
+      <c r="K103" s="15"/>
+      <c r="M103" s="34">
+        <v>45</v>
+      </c>
+      <c r="Q103" s="40">
+        <v>22</v>
+      </c>
+      <c r="R103" s="39">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A104" s="6">
+        <v>57</v>
+      </c>
+      <c r="B104" s="35">
+        <v>6</v>
+      </c>
+      <c r="C104" s="10"/>
+      <c r="D104" s="7">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="E104" s="11"/>
+      <c r="F104" s="11"/>
+      <c r="G104" s="11"/>
+      <c r="H104" s="29"/>
+      <c r="I104" s="11"/>
+      <c r="J104" s="14"/>
+      <c r="K104" s="15"/>
+      <c r="M104" s="34">
+        <v>46</v>
+      </c>
+      <c r="Q104" s="40">
+        <v>10</v>
+      </c>
+      <c r="R104" s="39">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A105" s="6">
+        <v>56</v>
+      </c>
+      <c r="B105" s="35">
+        <v>5</v>
+      </c>
+      <c r="C105" s="10"/>
+      <c r="D105" s="7">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="E105" s="11"/>
+      <c r="F105" s="11"/>
+      <c r="G105" s="11"/>
+      <c r="H105" s="29"/>
+      <c r="I105" s="11"/>
+      <c r="J105" s="14"/>
+      <c r="K105" s="15"/>
+      <c r="M105" s="34">
+        <v>47</v>
+      </c>
+      <c r="Q105" s="40">
+        <v>23</v>
+      </c>
+      <c r="R105" s="39">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A106" s="6">
+        <v>55</v>
+      </c>
+      <c r="B106" s="35">
+        <v>4</v>
+      </c>
+      <c r="C106" s="10"/>
+      <c r="D106" s="7">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="E106" s="11"/>
+      <c r="F106" s="11"/>
+      <c r="G106" s="11"/>
+      <c r="H106" s="29"/>
+      <c r="I106" s="11"/>
+      <c r="J106" s="14"/>
+      <c r="K106" s="15"/>
+      <c r="M106" s="34">
+        <v>48</v>
+      </c>
+      <c r="Q106" s="40">
+        <v>11</v>
+      </c>
+      <c r="R106" s="39">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A107" s="6">
+        <v>54</v>
+      </c>
+      <c r="B107" s="35">
+        <v>3</v>
+      </c>
+      <c r="C107" s="10"/>
+      <c r="D107" s="7">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="E107" s="11"/>
+      <c r="F107" s="11"/>
+      <c r="G107" s="11"/>
+      <c r="H107" s="29"/>
+      <c r="I107" s="11"/>
+      <c r="J107" s="14"/>
+      <c r="K107" s="15"/>
+      <c r="M107" s="34">
+        <v>49</v>
+      </c>
+      <c r="Q107" s="40">
+        <v>24</v>
+      </c>
+      <c r="R107" s="39">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A108" s="6">
+        <v>53</v>
+      </c>
+      <c r="B108" s="35">
+        <v>2</v>
+      </c>
+      <c r="C108" s="10"/>
+      <c r="D108" s="7">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="E108" s="11"/>
+      <c r="F108" s="11"/>
+      <c r="G108" s="11"/>
+      <c r="H108" s="29"/>
+      <c r="I108" s="11"/>
+      <c r="J108" s="14"/>
+      <c r="K108" s="15"/>
+      <c r="M108" s="34">
+        <v>50</v>
+      </c>
+      <c r="Q108" s="40">
+        <v>12</v>
+      </c>
+      <c r="R108" s="39">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A109" s="6">
+        <v>52</v>
+      </c>
+      <c r="B109" s="35">
+        <v>1</v>
+      </c>
+      <c r="C109" s="10"/>
+      <c r="D109" s="7">
+        <f>D108+1</f>
+        <v>99</v>
+      </c>
+      <c r="E109" s="11"/>
+      <c r="F109" s="11"/>
+      <c r="G109" s="11"/>
+      <c r="H109" s="29"/>
+      <c r="I109" s="11"/>
+      <c r="J109" s="14"/>
+      <c r="K109" s="15"/>
+      <c r="M109" s="34">
+        <v>51</v>
+      </c>
+      <c r="Q109" s="40">
+        <v>25</v>
+      </c>
+      <c r="R109" s="39">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A110" s="17"/>
+      <c r="B110" s="16"/>
+      <c r="C110" s="18"/>
+      <c r="D110" s="20"/>
+      <c r="E110" s="16"/>
+      <c r="F110" s="16"/>
+      <c r="G110" s="16"/>
+      <c r="H110" s="19"/>
+      <c r="I110" s="16"/>
+      <c r="J110" s="21"/>
+      <c r="K110" s="22"/>
+      <c r="L110" s="16"/>
+      <c r="M110" s="16"/>
+      <c r="N110" s="16"/>
+      <c r="O110" s="16"/>
+      <c r="P110" s="16"/>
+      <c r="Q110" s="36">
+        <v>13</v>
+      </c>
+      <c r="R110" s="16"/>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A111" s="17"/>
+      <c r="B111" s="16"/>
+      <c r="C111" s="18"/>
+      <c r="D111" s="37">
+        <f>D109+1</f>
+        <v>100</v>
+      </c>
+      <c r="E111" s="11"/>
+      <c r="F111" s="11"/>
+      <c r="G111" s="11"/>
+      <c r="H111" s="11"/>
+      <c r="I111" s="11"/>
+      <c r="J111" s="11"/>
+      <c r="K111" s="11"/>
+      <c r="L111" s="16"/>
+      <c r="M111" s="16"/>
+      <c r="N111" s="16"/>
+      <c r="O111" s="16"/>
+      <c r="P111" s="16"/>
+      <c r="Q111" s="16"/>
+      <c r="R111" s="16"/>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A112" s="12">
+        <v>49</v>
+      </c>
+      <c r="B112" s="35">
+        <v>49</v>
+      </c>
+      <c r="D112" s="16"/>
+      <c r="E112" s="16"/>
+      <c r="F112" s="16"/>
+      <c r="G112" s="16"/>
+      <c r="H112" s="16"/>
+      <c r="I112" s="16"/>
+      <c r="J112" s="16"/>
+      <c r="K112" s="16"/>
+      <c r="L112" s="16"/>
+      <c r="M112" s="16"/>
+      <c r="N112" s="16"/>
+      <c r="O112" s="16"/>
+      <c r="P112" s="16"/>
+      <c r="Q112" s="16"/>
+      <c r="R112" s="16"/>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A113" s="12">
+        <v>50</v>
+      </c>
+      <c r="B113" s="35">
+        <v>50</v>
+      </c>
+      <c r="D113" s="16"/>
+      <c r="E113" s="16"/>
+      <c r="F113" s="16"/>
+      <c r="G113" s="16"/>
+      <c r="H113" s="16"/>
+      <c r="I113" s="16"/>
+      <c r="J113" s="16"/>
+      <c r="K113" s="16"/>
+      <c r="L113" s="16"/>
+      <c r="M113" s="16"/>
+      <c r="N113" s="16"/>
+      <c r="O113" s="16"/>
+      <c r="P113" s="16"/>
+      <c r="Q113" s="16"/>
+      <c r="R113" s="16"/>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A114" s="12">
+        <v>51</v>
+      </c>
+      <c r="B114" s="35">
+        <v>51</v>
+      </c>
+      <c r="D114" s="16"/>
+      <c r="E114" s="16"/>
+      <c r="F114" s="16"/>
+      <c r="G114" s="16"/>
+      <c r="H114" s="16"/>
+      <c r="I114" s="16"/>
+      <c r="J114" s="16"/>
+      <c r="K114" s="16"/>
+      <c r="L114" s="16"/>
+      <c r="M114" s="16"/>
+      <c r="N114" s="16"/>
+      <c r="O114" s="16"/>
+      <c r="P114" s="16"/>
+      <c r="Q114" s="16"/>
+      <c r="R114" s="16"/>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A115" s="12">
+        <v>100</v>
+      </c>
+      <c r="C115" s="35">
+        <v>49</v>
+      </c>
+      <c r="D115" s="16"/>
+      <c r="E115" s="16"/>
+      <c r="F115" s="16"/>
+      <c r="G115" s="16"/>
+      <c r="H115" s="16"/>
+      <c r="I115" s="16"/>
+      <c r="J115" s="16"/>
+      <c r="K115" s="16"/>
+      <c r="L115" s="16"/>
+      <c r="M115" s="16"/>
+      <c r="N115" s="16"/>
+      <c r="O115" s="16"/>
+      <c r="P115" s="16"/>
+      <c r="Q115" s="16"/>
+      <c r="R115" s="16"/>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A116" s="12">
+        <v>101</v>
+      </c>
+      <c r="C116" s="35">
+        <v>50</v>
+      </c>
+      <c r="D116" s="16"/>
+      <c r="E116" s="16"/>
+      <c r="F116" s="16"/>
+      <c r="G116" s="16"/>
+      <c r="H116" s="16"/>
+      <c r="I116" s="16"/>
+      <c r="J116" s="16"/>
+      <c r="K116" s="16"/>
+      <c r="L116" s="16"/>
+      <c r="M116" s="16"/>
+      <c r="N116" s="16"/>
+      <c r="O116" s="16"/>
+      <c r="P116" s="16"/>
+      <c r="Q116" s="16"/>
+      <c r="R116" s="16"/>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A117" s="13">
+        <v>102</v>
+      </c>
+      <c r="C117" s="35">
+        <v>51</v>
+      </c>
+      <c r="D117" s="16"/>
+      <c r="E117" s="16"/>
+      <c r="F117" s="16"/>
+      <c r="G117" s="16"/>
+      <c r="H117" s="16"/>
+      <c r="I117" s="16"/>
+      <c r="J117" s="16"/>
+      <c r="K117" s="16"/>
+      <c r="L117" s="16"/>
+      <c r="M117" s="16"/>
+      <c r="N117" s="16"/>
+      <c r="O117" s="16"/>
+      <c r="P117" s="16"/>
+      <c r="Q117" s="16"/>
+      <c r="R117" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="45" orientation="portrait" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="111" max="16383" man="1"/>
+  </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="11" max="1048575" man="1"/>
   </colBreaks>

</xml_diff>